<commit_message>
Modified EV load growth python file to accurately output a smoothed .csv file for ev load each hour of the simulation period.
</commit_message>
<xml_diff>
--- a/inputs/EV_Load_Growth.xlsx
+++ b/inputs/EV_Load_Growth.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="5580" windowWidth="32260" windowHeight="12720" tabRatio="500"/>
+    <workbookView xWindow="1280" yWindow="280" windowWidth="32260" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Annual Load" sheetId="1" r:id="rId1"/>
@@ -216,9 +216,6 @@
     <t>PG&amp;E High</t>
   </si>
   <si>
-    <t>MW</t>
-  </si>
-  <si>
     <t>PG&amp;E Mid</t>
   </si>
   <si>
@@ -268,6 +265,9 @@
   </si>
   <si>
     <t>Administration</t>
+  </si>
+  <si>
+    <t>MWh</t>
   </si>
 </sst>
 </file>
@@ -375,6 +375,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PGE Load Growth Scenarios</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -398,6 +417,81 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Annual Load'!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2026.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2027.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2028.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2029.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2030.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2031.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2032.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2033.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2034.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Annual Load'!$B$2:$W$2</c:f>
@@ -492,6 +586,81 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Annual Load'!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2026.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2027.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2028.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2029.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2030.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2031.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2032.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2033.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2034.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Annual Load'!$B$3:$W$3</c:f>
@@ -586,6 +755,81 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Annual Load'!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2026.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2027.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2028.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2029.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2030.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2031.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2032.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2033.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2034.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Annual Load'!$B$4:$W$4</c:f>
@@ -680,6 +924,81 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Annual Load'!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2026.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2027.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2028.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2029.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2030.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2031.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2032.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2033.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2034.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Annual Load'!$B$5:$W$5</c:f>
@@ -774,6 +1093,81 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Annual Load'!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2026.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2027.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2028.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2029.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2030.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2031.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2032.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2033.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2034.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Annual Load'!$B$6:$W$6</c:f>
@@ -868,6 +1262,81 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Annual Load'!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2026.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2027.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2028.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2029.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2030.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2031.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2032.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2033.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2034.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Annual Load'!$B$7:$W$7</c:f>
@@ -962,6 +1431,81 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Annual Load'!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2026.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2027.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2028.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2029.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2030.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2031.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2032.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2033.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2034.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Annual Load'!$B$8:$W$8</c:f>
@@ -1056,6 +1600,81 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Annual Load'!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2026.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2027.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2028.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2029.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2030.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2031.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2032.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2033.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2034.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Annual Load'!$B$9:$W$9</c:f>
@@ -1150,6 +1769,81 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Annual Load'!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2026.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2027.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2028.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2029.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2030.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2031.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2032.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2033.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2034.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Annual Load'!$B$10:$W$10</c:f>
@@ -1244,6 +1938,81 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Annual Load'!$B$1:$W$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2021.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2022.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2023.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2025.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2026.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2027.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2028.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2029.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2030.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2031.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2032.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2033.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2034.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Annual Load'!$B$11:$W$11</c:f>
@@ -1331,20 +2100,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="594559704"/>
-        <c:axId val="595004584"/>
+        <c:axId val="681053288"/>
+        <c:axId val="680556648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="594559704"/>
+        <c:axId val="681053288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="595004584"/>
+        <c:crossAx val="680556648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1352,18 +2141,42 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="595004584"/>
+        <c:axId val="680556648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Annual Electric Vehicle</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Load (MWh)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="594559704"/>
+        <c:crossAx val="681053288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1697,11 +2510,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="111547912"/>
-        <c:axId val="586958808"/>
+        <c:axId val="681116376"/>
+        <c:axId val="681109496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111547912"/>
+        <c:axId val="681116376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1710,7 +2523,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="586958808"/>
+        <c:crossAx val="681109496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1718,7 +2531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="586958808"/>
+        <c:axId val="681109496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1729,7 +2542,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111547912"/>
+        <c:crossAx val="681116376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2075,11 +2888,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="718583432"/>
-        <c:axId val="606852808"/>
+        <c:axId val="681328808"/>
+        <c:axId val="681020056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="718583432"/>
+        <c:axId val="681328808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2088,7 +2901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="606852808"/>
+        <c:crossAx val="681020056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2096,7 +2909,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="606852808"/>
+        <c:axId val="681020056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2107,7 +2920,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="718583432"/>
+        <c:crossAx val="681328808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2477,11 +3290,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="680967464"/>
-        <c:axId val="560040200"/>
+        <c:axId val="567510920"/>
+        <c:axId val="720827960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="680967464"/>
+        <c:axId val="567510920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2490,7 +3303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="560040200"/>
+        <c:crossAx val="720827960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2498,7 +3311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="560040200"/>
+        <c:axId val="720827960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2509,7 +3322,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="680967464"/>
+        <c:crossAx val="567510920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2541,8 +3354,8 @@
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>768350</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -2996,14 +3809,14 @@
   <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B1">
         <v>2013</v>
@@ -3097,7 +3910,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2">
-        <f>2*8760</f>
+        <f t="shared" ref="B2:B7" si="1">2*8760</f>
         <v>17520</v>
       </c>
       <c r="C2" s="2">
@@ -3187,10 +4000,10 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <f>2*8760</f>
+        <f t="shared" si="1"/>
         <v>17520</v>
       </c>
       <c r="C3">
@@ -3280,10 +4093,10 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <f>2*8760</f>
+        <f t="shared" si="1"/>
         <v>17520</v>
       </c>
       <c r="C4">
@@ -3373,10 +4186,10 @@
     </row>
     <row r="5" spans="1:23" s="2" customFormat="1">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
-        <f>2*8760</f>
+        <f t="shared" si="1"/>
         <v>17520</v>
       </c>
       <c r="C5" s="2">
@@ -3466,10 +4279,10 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <f>2*8760</f>
+        <f t="shared" si="1"/>
         <v>17520</v>
       </c>
       <c r="C6">
@@ -3559,10 +4372,10 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <f>2*8760</f>
+        <f t="shared" si="1"/>
         <v>17520</v>
       </c>
       <c r="C7">
@@ -3652,7 +4465,7 @@
     </row>
     <row r="8" spans="1:23" s="2" customFormat="1">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
         <f>'2013 PGE Projections'!E2*8760</f>
@@ -3745,7 +4558,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2">
         <f>'2013 PGE Projections'!E3*8760</f>
@@ -3838,7 +4651,7 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <f>'2013 PGE Projections'!E4*8760</f>
@@ -3931,7 +4744,7 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <f>2*8760</f>
@@ -4038,8 +4851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4691,17 +5504,17 @@
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1">
         <v>2008</v>
@@ -4813,7 +5626,7 @@
     </row>
     <row r="2" spans="1:29">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <f>50/12</f>
@@ -4929,7 +5742,7 @@
     </row>
     <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <f>25/12</f>
@@ -5045,7 +5858,7 @@
     </row>
     <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <f>5/12</f>
@@ -5183,7 +5996,7 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1">
         <v>2010</v>
@@ -5193,7 +6006,7 @@
         <v>2011</v>
       </c>
       <c r="D1">
-        <f t="shared" ref="D1:AO1" si="0">C1+1</f>
+        <f t="shared" ref="D1:Z1" si="0">C1+1</f>
         <v>2012</v>
       </c>
       <c r="E1">
@@ -5290,7 +6103,7 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -5393,7 +6206,7 @@
     </row>
     <row r="3" spans="1:27">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5496,7 +6309,7 @@
     </row>
     <row r="4" spans="1:27">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5614,14 +6427,14 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1">
         <v>2011</v>
@@ -5721,7 +6534,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <f>250000/10</f>
@@ -5829,7 +6642,7 @@
         <v>2.4</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:K4" si="2">D2/C2</f>
+        <f t="shared" ref="D3:K3" si="2">D2/C2</f>
         <v>2.5</v>
       </c>
       <c r="E3">

</xml_diff>